<commit_message>
update sql query and output comparison
</commit_message>
<xml_diff>
--- a/test_results_sql.xlsx
+++ b/test_results_sql.xlsx
@@ -1,37 +1,389 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/neo/Desktop/DataWorksAI/text2sql_prod/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25CCCF2B-98F7-FE4C-A898-A41DA2DE9341}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="57">
+  <si>
+    <t>Question</t>
+  </si>
+  <si>
+    <t>Expected SQL</t>
+  </si>
+  <si>
+    <t>Generated SQL</t>
+  </si>
+  <si>
+    <t>Expected Output</t>
+  </si>
+  <si>
+    <t>Generated Output</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>List the colleges where men's admission are more than women's admissions</t>
+  </si>
+  <si>
+    <t>SELECT ic.pcinstnm
+FROM ic2022campuses ic
+JOIN adm2022 a ON ic.unitid = a.unitid
+WHERE a.admcon1 &gt; a.admcon2;</t>
+  </si>
+  <si>
+    <t>SELECT a.unitid
+FROM adm2022 a
+WHERE a.applcnm &gt; a.applcnw;</t>
+  </si>
+  <si>
+    <t>The colleges where men's admissions are more than women's admissions are Harding School of Theology, Mayo Clinic College of Medicine and Science - Florida, Mayo Clinic College of Medicine and Science - Arizona, and Jamestown Business College.</t>
+  </si>
+  <si>
+    <t>The colleges where men's admissions are more than women's admissions are those with the corresponding unitid values from the SQL result.</t>
+  </si>
+  <si>
+    <t>Show institutions with the highest number of applicants</t>
+  </si>
+  <si>
+    <t>SELECT ic.pcinstnm, a.applcn
+FROM adm2022 a
+JOIN ic2022campuses ic ON a.unitid = ic.unitid
+ORDER BY a.applcn DESC
+LIMIT 3;</t>
+  </si>
+  <si>
+    <t>SELECT unitid, applcn
+FROM adm2022
+ORDER BY applcn DESC
+LIMIT 3;</t>
+  </si>
+  <si>
+    <t>The institutions with the highest number of applicants are:
+1. San Diego State University-Imperial Valley Campus with 77,250 applicants
+2. Arizona State University-Polytechnic with 68,789 applicants
+3. Arizona State University-West with 68,789 applicants</t>
+  </si>
+  <si>
+    <t>The institutions with the highest number of applicants are:
+1. Institution with unitid 110662 has 149,801 applicants
+2. Institution with unitid 110680 has 131,197 applicants
+3. Institution with unitid 110635 has 128,209 applicants</t>
+  </si>
+  <si>
+    <t>Retrieve colleges with a completion of college-preparatory program percentage
+between 50% and 70%</t>
+  </si>
+  <si>
+    <t>SELECT ic.pcinstnm
+FROM adm2022 a
+JOIN ic2022campuses ic ON a.unitid = ic.unitid
+WHERE a.admcon4 BETWEEN 50 AND 70;
+LIMIT 3;</t>
+  </si>
+  <si>
+    <t>SELECT unitid
+FROM adm2022
+WHERE admcon4 &gt;= 50 AND admcon4 &lt;= 70;</t>
+  </si>
+  <si>
+    <t>The error in the SQL query is due to the incorrect placement of the "LIMIT 3;" statement. It should be placed at the end of the query after the WHERE clause. Here is the corrected SQL query:
+SELECT ic.pcinstnm
+FROM adm2022 a
+JOIN ic2022campuses ic ON a.unitid = ic.unitid
+WHERE a.admcon4 BETWEEN 50 AND 70
+LIMIT 3;
+This query will retrieve colleges with a completion of college-preparatory program percentage between 50% and 70% and limit the results to 3 rows.</t>
+  </si>
+  <si>
+    <t>The SQL query retrieves the unitid of colleges with a completion of college-preparatory program percentage between 50% and 70%.</t>
+  </si>
+  <si>
+    <t>Find institutions with more women applicants than men applicants, but a higher 
+admission rate for men applicants compared to women applicants.</t>
+  </si>
+  <si>
+    <t>SELECT ic.pcinstnm
+FROM ic2022campuses ic
+JOIN adm2022 a ON ic.unitid = a.unitid
+WHERE a.applcnw &gt; a.applcn
+AND a.admcon2 &gt; a.admcon1;</t>
+  </si>
+  <si>
+    <t>SELECT a.instnm
+FROM adm2022 a
+JOIN (
+    SELECT unitid,
+           SUM(CASE WHEN applcnm &gt; applcnw THEN 1 ELSE 0 END) AS more_men_applicants,
+           SUM(CASE WHEN applcnm &gt; applcnw AND (admssnm::FLOAT / applcnm) &gt; (admssnw::FLOAT / applcnw) THEN 1 ELSE 0 END) AS higher_adm_rate_men
+    FROM adm2022
+    GROUP BY unitid
+) b ON a.unitid = b.unitid
+WHERE b.more_men_applicants &gt; 0 AND b.higher_adm_rate_men &gt; 0;</t>
+  </si>
+  <si>
+    <t>The SQL query provided is looking for institutions where the number of women applicants is greater than the number of men applicants, and the admission rate for men applicants is higher than the admission rate for women applicants. The SQL result will display the names of these institutions.</t>
+  </si>
+  <si>
+    <t>The error in the SQL query is due to the fact that the column "instnm" does not exist in the table or result set. To fix this error, you should remove the reference to "a.instnm" in the SELECT statement and only select the columns that are present in the result set or tables being queried.</t>
+  </si>
+  <si>
+    <t>Find institutions with a high number of applicants, but a lower admission rate for 
+legacy applicants compared to non-legacy applicants</t>
+  </si>
+  <si>
+    <t>SELECT ic.pcinstnm, a.applcn, a.admssn, a.applcnm, a.applcnw, a.admssnm, a.admssnw
+FROM a.adm2022
+JOIN ic2022campuses ic on a.UNITID = ic.UNITID
+WHERE a.applcn &gt; 1000
+AND (a.admssnm::numeric / a.applcnm::numeric) &lt; (a.admssnw::numeric / a.applcnw::numeric);</t>
+  </si>
+  <si>
+    <t>SELECT a.unitid, a.admcon12 AS total_applicants, a.admcon17 AS total_admissions,
+    (a.admcon17::NUMERIC / NULLIF(a.admcon12, 0)) AS admission_rate,
+    b.admcon11 AS legacy_status
+FROM adm2022 a
+JOIN adm2022 b ON a.unitid = b.unitid
+WHERE a.admcon12 &gt; 5000
+AND b.admcon11 = 1
+AND (a.admcon17::NUMERIC / NULLIF(a.admcon12, 0)) &lt; (b.admcon17::NUMERIC / NULLIF(b.admcon12, 0));</t>
+  </si>
+  <si>
+    <t>The error message indicates that the table "a.adm2022" does not exist in the database. This could be due to a typo in the table name or the table not being created in the database. To resolve this issue, you should check the database schema to ensure that the table "a.adm2022" exists and is spelled correctly. If the table does not exist, you may need to create it or modify the query to reference the correct table that contains the data you are looking for.</t>
+  </si>
+  <si>
+    <t>The error in the SQL query is due to the column `a.admcon17` not existing in the table `adm2022`. This error is preventing the query from executing successfully and providing the desired result. To fix this issue, you need to check the column names in the `adm2022` table and make sure they are correctly referenced in the query.</t>
+  </si>
+  <si>
+    <t>List colleges where the number of admissions is significantly higher than the number 
+of applicants, in California</t>
+  </si>
+  <si>
+    <t>SELECT ic.pcinstnm
+FROM adm2022 a
+JOIN c2022dep c ON a.unitid = c.unitid
+JOIN ic2022campuses ic ON a.unitid = ic.unitid
+WHERE a.admssn &gt; a.applcn
+AND c.cipcode = 6.0;</t>
+  </si>
+  <si>
+    <t>SELECT a.unitid
+FROM adm2022 a
+JOIN c2022dep c ON a.unitid = c.unitid
+WHERE a.admssn &gt; a.applcn
+AND c.unitid IN (
+    SELECT unitid
+    FROM hd2022
+    WHERE stabbr = 'CA'
+);</t>
+  </si>
+  <si>
+    <t>The SQL query provided lists colleges in California where the number of admissions is significantly higher than the number of applicants.</t>
+  </si>
+  <si>
+    <t>The SQL query provided will list colleges in California where the number of admissions is significantly higher than the number of applicants.</t>
+  </si>
+  <si>
+    <t>list the college names with high admissions</t>
+  </si>
+  <si>
+    <t>SELECT ic.pcinstnm
+FROM adm2022 a
+JOIN ic2022campuses ic ON a.UNITID = ic.UNITID
+WHERE a.admssn &gt; 5000;</t>
+  </si>
+  <si>
+    <t>SELECT instnm
+FROM adm2022
+ORDER BY admssn DESC;</t>
+  </si>
+  <si>
+    <t>The college names with high admissions (admissions greater than 5000) are:
+1. Troy University-Phenix City Campus
+2. Troy University-Montgomery Campus
+3. Troy University-Dothan Campus
+4. Troy University-Online
+5. Troy University-Support Sites
+6. Arizona State University-West
+7. Arizona State University-Polytechnic
+8. Arizona State University-Downtown Phoenix
+9. Arizona State University - Tucson
+10. Arizona State University - Lake Havasu
+11. Arizona State University - The Gila Valley
+12. Arizona State University - Yuma
+13. Arizona State University - Pinal
+14. Arizona State University - Cochise
+15. Arizona State University - Yavapai
+16. Arizona State University - Pima
+17. Arizona State University - Washington, D0C0
+18. Arizona State University - Northeastern Arizona
+19. Arizona State University - Mesa City Center
+20. San Diego State University-Imperial Valley Campus
+21. Jesuit School of Theology of Santa Clara University
+22. Barry University Law School
+23. University of Maine - Machias
+24. University of Mississippi Medical Center
+25. The University of Montana - Missoula College
+26. Monmouth University - Monmouth Park Corporate Center
+27. Clarkson University Capital Region Campus
+28. CUNY Brooklyn College - Feirstein Graduate School of Cinema
+29. Pratt Manhattan-A Division of Pratt Institute
+30. Saint John's University - Staten Island Campus
+31. Washington State University-Vancouver
+32. Washington State University-Spokane
+33. Washington State University-Tri Cities
+34. Washington State University - Everett Campus
+35. Purdue University - Purdue Polytechnic Anderson
+36. Purdue University - Purdue Polytechnic Indianapolis
+37. Purdue University - Purdue Polytechnic South Bend
+38. Purdue University - Purdue Polytechnic New Albany
+39. Purdue University - Purdue Polytechnic Columbus
+40. Purdue University - Purdue Polytechnic Kokomo
+41. Purdue University - Purdue Polytechnic Richmond
+42. Purdue University - Purdue Polytechnic Lafayette
+43. Purdue University - Purdue Polytechnic Vincennes
+44. Purdue University - Westgate Academy</t>
+  </si>
+  <si>
+    <t>The error occurred because the column "instnm" does not exist in the table "adm2022". Please check the column names in the table and adjust the SQL query accordingly to retrieve the college names with high admissions.</t>
+  </si>
+  <si>
+    <t>list institutions in washington with good performance</t>
+  </si>
+  <si>
+    <t>SELECT ic.pcinstnm
+FROM hd2022 h
+JOIN ic2022campuses ic
+ON h.UNITID = ic.UNITID
+WHERE stabbr = 'WA';</t>
+  </si>
+  <si>
+    <t>SELECT hd.instnm
+FROM hd2022 hd
+JOIN gr2022 gr ON hd.unitid = gr.unitid
+WHERE hd.stabbr = 'WA'
+AND gr.chrtstat = 1;</t>
+  </si>
+  <si>
+    <t>The institutions in Washington with good performance are:
+1. Shoreline Community College - CNC Machinists Program , Georgetown SSC
+2. Washington State University-Vancouver
+3. Washington State University-Spokane
+4. Washington State University-Tri Cities
+5. Washington State University - Everett Campus</t>
+  </si>
+  <si>
+    <t>The SQL query provided lists the institutions in Washington with good performance.</t>
+  </si>
+  <si>
+    <t>List colleges with most applicants</t>
+  </si>
+  <si>
+    <t>SELECT ic.pcinstnm
+FROM adm2022 a
+JOIN ic2022campuses ic
+ON ic.UNITID = a.UNITID
+ORDER BY a.applcn DESC</t>
+  </si>
+  <si>
+    <t>SELECT unitid, applcn
+FROM adm2022
+ORDER BY applcn DESC;</t>
+  </si>
+  <si>
+    <t>The colleges with the most applicants based on the SQL query and result provided are:
+1. San Diego State University-Imperial Valley Campus
+2. Arizona State University - Yavapai
+3. Arizona State University-West
+4. Arizona State University-Polytechnic
+5. Arizona State University-Downtown Phoenix
+These are the top 5 colleges with the highest number of applicants.</t>
+  </si>
+  <si>
+    <t>The colleges with the most applicants based on the SQL query and result are as follows:
+1. College with unitid 110662 has 149,801 applicants.
+2. College with unitid 110680 has 131,197 applicants.
+3. College with unitid 110635 has 128,209 applicants.
+4. College with unitid 110653 has 119,191 applicants.
+5. College with unitid 110705 has 110,995 applicants.
+These are the top 5 colleges with the most applicants based on the data provided.</t>
+  </si>
+  <si>
+    <t>Find institutions with a significant difference between the number of male and female 
+applicants, but a similar admission rate for both genders</t>
+  </si>
+  <si>
+    <t>SELECT ic.pcinstnm
+FROM adm2022 a
+JOIN ic2022campuses ic
+ON ic.UNITID = a.UNITID
+WHERE ABS(a.applcnm - a.applcnw) &gt; 500
+AND ABS((a.admssnm::numeric / a.applcnm::numeric) - (a.admssnw::numeric / a.applcnw::numeric)) &lt; 0.05;</t>
+  </si>
+  <si>
+    <t>SELECT a.instnm
+FROM adm2022 a
+JOIN c2022dep c ON a.unitid = c.unitid
+WHERE (a.applcnm - a.applcnw) &gt; 1000
+AND ABS((a.admssnm::NUMERIC / a.applcnm) - (a.admssnw::NUMERIC / a.applcnw)) &lt; 0.05;</t>
+  </si>
+  <si>
+    <t>The institutions listed in the SQL result have a significant difference between the number of male and female applicants (more than 500 difference), but a similar admission rate for both genders (difference less than 5%).</t>
+  </si>
+  <si>
+    <t>The error in the SQL query is due to the fact that the column "instnm" does not exist in the tables being referenced (adm2022 and c2022dep). To fix this error, you need to identify the correct column that contains the institution names and replace "a.instnm" with the appropriate column name in the SELECT statement.</t>
+  </si>
+  <si>
+    <t>Output Incorrect</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -46,93 +398,50 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
+  <cellXfs count="5">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -420,65 +729,241 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="47" customWidth="1"/>
+    <col min="2" max="2" width="36" customWidth="1"/>
+    <col min="3" max="3" width="38.5" customWidth="1"/>
+    <col min="4" max="4" width="53" customWidth="1"/>
+    <col min="5" max="5" width="43.5" customWidth="1"/>
+    <col min="6" max="6" width="16.1640625" style="3" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Question</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Expected SQL</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Generated SQL</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Status</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>how many colleges in Boston</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>SELECT COUNT(*) 
-FROM hd2022 
-WHERE city = 'Boston';</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>SELECT COUNT(*) 
-FROM hd2022 
-WHERE city = 'Boston';</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Correct</t>
-        </is>
+    <row r="1" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="128" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="208" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="240" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="224" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="144" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="112" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="176" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="128" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>